<commit_message>
feat: reduce weight of brick to make model more reasonable
NEEDS TO BE UPDATED
</commit_message>
<xml_diff>
--- a/references/background_data/b2-b5.xlsx
+++ b/references/background_data/b2-b5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE24774-4C5E-4BD0-A7A1-E3846C891148}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AF3B39-0A72-410C-9DD6-868788590BC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="1">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>